<commit_message>
feat(backend): complete product scraping
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,26 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>brand</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rating</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>img_url</t>
         </is>
       </c>
@@ -443,154 +463,864 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/11948318/2022/3/4/a16375d2-a672-4cbc-9a7b-131c2176d2a41646394283494-Roadster-Men-Grey-Melange-Solid-Round-Neck-T-shirt-801164639-1.jpg</t>
+          <t>Men Pure Cotton Polo T-shirt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>U.S. Polo Assn.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rs. 1279</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/19023024/2022/8/2/136b1ddb-e498-4e85-b9a6-4dbe4f0ae2821659421677365-US-Polo-Assn-Men-Tshirts-5691659421676904-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/19023024/2022/8/2/136b1ddb-e498-4e85-b9a6-4dbe4f0ae2821659421677365-US-Polo-Assn-Men-Tshirts-5691659421676904-1.jpg</t>
+          <t>Printed Cotton Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Moda Rapido</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rs. 295</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2378362/2018/6/9/270e0a7e-365b-4640-9433-b269c60bf3061528527188563-Moda-Rapido-Men-Maroon-Printed-Round-Neck-T-shirt-3811528527-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2378362/2018/6/9/270e0a7e-365b-4640-9433-b269c60bf3061528527188563-Moda-Rapido-Men-Maroon-Printed-Round-Neck-T-shirt-3811528527-1.jpg</t>
+          <t>Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Rs. 199</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2275365/2019/9/10/4f24f563-c764-4f27-9fc5-9ad3dcf167621568108715062-Roadster-Men-White-Solid-Round-Neck-T-shirt-1641568108713591-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2275365/2019/9/10/4f24f563-c764-4f27-9fc5-9ad3dcf167621568108715062-Roadster-Men-White-Solid-Round-Neck-T-shirt-1641568108713591-1.jpg</t>
+          <t>Men Polo Collar T-shirt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ONN</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Rs. 599</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18995934/2022/7/6/5a241a63-0047-4546-8640-05b0d78e62d11657120401052MensPeacockBlueSolidPoloCollarT-Shirt6.jpg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18995934/2022/7/6/5a241a63-0047-4546-8640-05b0d78e62d11657120401052MensPeacockBlueSolidPoloCollarT-Shirt6.jpg</t>
+          <t>Men Polo Collar T-shirt</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Louis Philippe Sport</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Rs. 766</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18762302/2022/6/29/e4865577-1370-4ede-a5b9-325bf48b6c931656501603337-Louis-Philippe-Sport-Men-Brown-Polo-Collar-Slim-Fit-T-shirt--1.jpg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18762302/2022/6/29/e4865577-1370-4ede-a5b9-325bf48b6c931656501603337-Louis-Philippe-Sport-Men-Brown-Polo-Collar-Slim-Fit-T-shirt--1.jpg</t>
+          <t>Men Solid Oversized Cotton</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Difference of Opinion</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Rs. 558</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/16407468/2021/12/28/fce7ca1e-01ec-4c12-a90f-c7b75abda0e01640669480687-Difference-of-Opinion-Men-Tshirts-4021640669480120-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/16407468/2021/12/28/fce7ca1e-01ec-4c12-a90f-c7b75abda0e01640669480687-Difference-of-Opinion-Men-Tshirts-4021640669480120-1.jpg</t>
+          <t>Typography Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Rs. 239</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2308267/2018/1/29/11517216335231-Roadster-Men-Maroon-Printed-Round-Neck-T-shirt-5591517216335098-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2308267/2018/1/29/11517216335231-Roadster-Men-Maroon-Printed-Round-Neck-T-shirt-5591517216335098-1.jpg</t>
+          <t>Typography Print T-shirt</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Huetrap</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Rs. 472</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/productimage/2019/12/12/1aab2a18-6774-4f83-b292-fe301755a3351576102551329-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/productimage/2019/12/12/1aab2a18-6774-4f83-b292-fe301755a3351576102551329-1.jpg</t>
+          <t>Men Colourblocked Polo Collar Slim Fit T-shirt</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>U.S. Polo Assn.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Rs. 1999</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/19022900/2022/8/2/5c64d048-1cc0-40cf-be74-f1e1243202ec1659421887623-US-Polo-Assn-Men-Tshirts-7651659421887232-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/19022900/2022/8/2/5c64d048-1cc0-40cf-be74-f1e1243202ec1659421887623-US-Polo-Assn-Men-Tshirts-7651659421887232-1.jpg</t>
+          <t>Solid Round Neck T-shirt</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Rs. 189</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/10384501/2020/11/6/f8a9d333-d5fb-45e6-8d4e-b426a65615131604640103374-Roadster-Men-Charcoal-Solid-Round-Neck-T-shirt-3841604640101-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/10384501/2020/11/6/f8a9d333-d5fb-45e6-8d4e-b426a65615131604640103374-Roadster-Men-Charcoal-Solid-Round-Neck-T-shirt-3841604640101-1.jpg</t>
+          <t>Slim Tropical Printed Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Urbano Fashion</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Rs. 494</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/12377258/2020/9/11/ce1b7bcb-a65a-4eb0-a317-42ac02718f1e1599798741705UrbanoFashionPrintedMenRoundNeckDarkGreenT-Shirt1.jpg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/12329076/2020/9/14/04dcacfe-ef3a-4c1e-bf49-a8baea36305c1600060557950-WROGN-Men-Tshirts-8461600060554845-1.jpg</t>
+          <t>Henley Cotton Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>HIGHLANDER</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Rs. 384</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1703254/2018/4/3/11522748461209-HIGHLANDER-Men-Navy-Blue-Solid-Henley-Neck-T-Shirt-1731522748461015-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2330211/2019/2/1/3cbc81a0-dfcb-4a51-adb9-c02b87d1d4cd1549002838431-Roadster-Men-White-Solid-T-shirt-981549002836084-1.jpg</t>
+          <t>Time Travlr Round Neck Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Rs. 279</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2340658/2018/4/20/11524220878763-Roadster-Men-Navy-Blue-Printed-Round-Neck-T-shirt-1941524220878618-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18995986/2022/7/6/940556c0-8b8b-4d21-937b-4f9ae9c0b6bc1657120812072MensFluorescentGreenSolidPoloCollarT-Shirt5.jpg</t>
+          <t>Men Solid Polo Collar T-shirt</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Rs. 1034</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18656682/2022/6/7/a672f1b8-9c3e-4f25-97d4-d4abebb6e7541654595626340AllenSollyBlueTShirt1.jpg</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/19024164/2022/7/19/7e42f78b-1464-412d-892a-4e1382d8ecb11658208852520-Blackberrys-Men-Black-Polo-Collar-T-shirt-8151658208852109-1.jpg</t>
+          <t>Printed Polo Collar T-shirt</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BULLMER</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Rs. 529</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/productimage/2021/1/15/a930706f-99b8-4f13-974b-7628fe5280c91610704104668-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1894413/2017/6/20/11497943671766-WROGN-Men-Grey-Melange-Self-Design-Round-Neck-T-shirt-881497943671356-1.jpg</t>
+          <t>Colourblocked Cotton Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Campus Sutra</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Rs. 398</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/10016983/2019/6/20/b5caaca7-b5e8-4134-9283-65473a2388031561026348090-Campus-Sutra-Men-Blue-Colourblocked-Round-Neck-T-shirt-99915-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1703254/2018/4/3/11522748461209-HIGHLANDER-Men-Navy-Blue-Solid-Henley-Neck-T-Shirt-1731522748461015-1.jpg</t>
+          <t>Men Polo Collar Applique T-shirt</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ONN</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Rs. 599</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18992828/2022/7/24/99256e92-3db0-4538-a033-57acad0698761658643788806ONNMenFluorescentGreenPoloCollarAppliqueT-shirt1.jpg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18996024/2022/7/6/318d72f3-fbcc-48e9-9d29-b5f9b371739e1657120808059MensPurpleSolidPoloCollarT-Shirt6.jpg</t>
+          <t>Solid Round Neck Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>HIGHLANDER</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Rs. 349</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1703238/2018/3/30/11522394076063-HIGHLANDER-Men-Black-Solid-Round-Neck-T-shirt-4731522394075913-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2340658/2018/4/20/11524220878763-Roadster-Men-Navy-Blue-Printed-Round-Neck-T-shirt-1941524220878618-1.jpg</t>
+          <t>Men Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Levis</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Rs. 959</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18984180/2022/7/27/ed26fae0-b00b-4645-8550-71eba6d77ce81658920876978-Levis-Men-Green-Brand-Logo-Printed-Pure-Cotton-T-shirt-36816-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18656682/2022/6/7/a672f1b8-9c3e-4f25-97d4-d4abebb6e7541654595626340AllenSollyBlueTShirt1.jpg</t>
+          <t>Men Camouflage Printed Loose T-shirt</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>VEIRDO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Rs. 549</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/17868156/2022/4/12/4084bedc-aa91-40c8-bed9-e8e74bbdd5f31649779743002VEIRDOMenWhiteCamouflagePrintedMonochromeLooseT-shirt1.jpg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/productimage/2021/1/15/a930706f-99b8-4f13-974b-7628fe5280c91610704104668-1.jpg</t>
+          <t>Polo Collar T-shirt</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FIDO DIDO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Rs. 644</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2471500/2018/2/9/11518159758071-FIDO-DIDO-Men-Tshirts-9591518159757862-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/10016983/2019/6/20/b5caaca7-b5e8-4134-9283-65473a2388031561026348090-Campus-Sutra-Men-Blue-Colourblocked-Round-Neck-T-shirt-99915-1.jpg</t>
+          <t>Drop Shoulder Longline T-shirt</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Rs. 399</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1824339/2022/4/18/ff4c8434-9e4f-4d11-9f1e-448cebdb5c6b1650284989788RoadsterMenBlackDrop-ShoulderLonglineT-shirt1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Printed Round Neck T-shirt</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>HIGHLANDER</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Rs. 219</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/productimage/2021/3/10/33b84eef-8837-42b0-983a-ac43a0eb182e1615358243811-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Solid Round Neck Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Rs. 249</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/12504580/2020/12/18/383f3313-627b-4f06-bc1c-e4153b5669e11608284567024-Roadster-Men-Tshirts-141608284566088-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Men Typography Printed Slim Fit T-shirt</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Tommy Hilfiger</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Rs. 1199</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/16363924/2022/7/27/59ad6fc7-5d84-4ebc-9483-702b3273a00f1658920851286TommyHilfigerMenBlackTypographyPrintedSlimFitT-shirt1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Polo Collar Cotton Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Rs. 404</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2483671/2018/5/18/fe21cc3a-c7de-4374-b140-6d9d36fecfb41526629339145-Roadster-Men-Grey-Melange-Solid-Polo-Collar-T-shirt-5041526629336751-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Men Solid Slim Fit T-shirt</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>WROGN</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Rs. 769</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/15069722/2021/10/19/eb622605-80d3-429e-b278-5d6b12277f8b1634637202987-WROGN-Men-Tshirts-8181634637202468-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Men Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Louis Philippe Jeans</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Rs. 766</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/15203074/2021/9/8/c708ac57-1634-4dd7-85f1-17a94a414cac1631084900361-Louis-Philippe-Jeans-Men-Tshirts-2461631084899784-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Varsity Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Rs. 419</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/2303701/2019/3/7/dcb5e566-c7ab-4e0e-bdfb-66d93d7932901551949925470-Roadster-Men-Navy-Blue-Printed-Round-Neck-T-shirt-1471551949-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Manchester United T-shirt</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ADIDAS</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Rs. 2649</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/14790112/2021/8/9/e6400d90-3bcb-4e3c-aaa4-a581a88cc2b11628494509668-ADIDAS-Men-Tshirts-6861628494509162-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Men Brand Logo Printed T-shirt</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Levis</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Rs. 959</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/18984042/2022/7/27/4761bb29-e98e-4074-8da8-928db92d03031658919936961-Levis-Men-White-Brand-Logo-Printed-Pure-Cotton-T-shirt-68816-1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Striped Polo Pure Cotton T-shirt</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Rs. 480</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://assets.myntassets.com/dpr_2,q_60,w_210,c_limit,fl_progressive/assets/images/1751640/2017/5/15/11494837350088-Roadster-Men-White-Striped-Polo-Collar-T-shirt-7621494837349847-1.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>